<commit_message>
Game solution tests finished and pass
</commit_message>
<xml_diff>
--- a/TestsShownClueLayout.xlsx
+++ b/TestsShownClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torigeis/306/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torigeis/306/ClueGame2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC6B323-8AE4-924D-AE93-AA581C76C403}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FDF1DC-57E6-5248-A7AF-4F17CDF80354}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14120" yWindow="1360" windowWidth="24280" windowHeight="13720" xr2:uid="{58782FFD-F989-B54E-B586-FC3BAB022337}"/>
+    <workbookView xWindow="10220" yWindow="2620" windowWidth="24280" windowHeight="13720" xr2:uid="{58782FFD-F989-B54E-B586-FC3BAB022337}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
   <dimension ref="B2:AD28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,11 +735,11 @@
       <c r="O3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>4</v>
+      <c r="P3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>6</v>
@@ -1336,8 +1336,8 @@
       <c r="V11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="W11" s="3" t="s">
-        <v>4</v>
+      <c r="W11" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.2">
@@ -1956,8 +1956,8 @@
       <c r="B21">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>4</v>
+      <c r="C21" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>7</v>
@@ -2444,8 +2444,8 @@
       <c r="F28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>4</v>
+      <c r="G28" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>5</v>

</xml_diff>